<commit_message>
Committed on 03/02/2022 at 15:05
</commit_message>
<xml_diff>
--- a/data/testscriptdata.xlsx
+++ b/data/testscriptdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORKSTATION\JAVA\comcast_selenium_framework\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORKSTATION\SELENIUM\Vtiger_Automation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98DCF0C-41F6-4E33-BC4C-BEBE934A3E1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4E442D-70F5-4AE1-A2A6-E32B4ABC78D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Org" sheetId="1" r:id="rId1"/>
@@ -26,14 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>OrgName</t>
   </si>
   <si>
-    <t>Rohit</t>
-  </si>
-  <si>
     <t>Last Name</t>
   </si>
   <si>
@@ -56,13 +53,40 @@
   </si>
   <si>
     <t>Self Generated</t>
+  </si>
+  <si>
+    <t>Agro Tech Food Ltd</t>
+  </si>
+  <si>
+    <t>Food &amp; Beverage</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Investor</t>
+  </si>
+  <si>
+    <t>Mahindra &amp; Mahindra</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>Integrator</t>
+  </si>
+  <si>
+    <t>Resilient Innovation Pvt Ltd</t>
+  </si>
+  <si>
+    <t>Technology</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -85,6 +109,17 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -106,10 +141,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,31 +461,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
+    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -456,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F8892F-B6BF-48AD-9250-6E7F04AB9741}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,30 +542,30 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>